<commit_message>
update test_kpi, all avaiable kpi functions passed
</commit_message>
<xml_diff>
--- a/energy_flexibility_kpis/test/data1_simple.xlsx
+++ b/energy_flexibility_kpis/test/data1_simple.xlsx
@@ -1,6 +1,6 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" mc:Ignorable="x15 xr xr6 xr10">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25928"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
@@ -8,20 +8,33 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\repo\contribute_energy_flexibility_kpis\develop_test\energy_flexibility_kpis\test\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:40009_{0EF8D686-84A9-4D7C-9EAF-081C775B3139}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C4DC4B3F-9C8D-4536-983C-F37121FFFAD1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="15720" activeTab="1"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="data1_simple" sheetId="1" r:id="rId1"/>
     <sheet name="flexibility factor" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="3">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="11">
   <si>
     <t>timestamp</t>
   </si>
@@ -31,11 +44,38 @@
   <si>
     <t>flexible_power</t>
   </si>
+  <si>
+    <t>mean</t>
+  </si>
+  <si>
+    <t>peak</t>
+  </si>
+  <si>
+    <t>peak_demand_reduction</t>
+  </si>
+  <si>
+    <t>LF</t>
+  </si>
+  <si>
+    <t>FF</t>
+  </si>
+  <si>
+    <t>KPI need ref</t>
+  </si>
+  <si>
+    <t>building_energy_flexibility_index</t>
+  </si>
+  <si>
+    <t>peak energy</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <numFmts count="1">
+    <numFmt numFmtId="166" formatCode="0.0000"/>
+  </numFmts>
   <fonts count="18" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -172,7 +212,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="33">
+  <fills count="34">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -352,8 +392,14 @@
         <bgColor indexed="65"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="10">
+  <borders count="18">
     <border>
       <left/>
       <right/>
@@ -465,6 +511,86 @@
       </top>
       <bottom style="double">
         <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color rgb="FFFF0000"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FFFF0000"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color rgb="FFFF0000"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color rgb="FFFF0000"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color rgb="FFFF0000"/>
+      </right>
+      <top style="thin">
+        <color rgb="FFFF0000"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FFFF0000"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color rgb="FFFF0000"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FFFF0000"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color rgb="FFFF0000"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color rgb="FFFF0000"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color rgb="FFFF0000"/>
       </bottom>
       <diagonal/>
     </border>
@@ -513,9 +639,19 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="22" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
+    <xf numFmtId="22" fontId="0" fillId="33" borderId="11" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="14" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="16" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1"/>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -870,11 +1006,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C25"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:K25"/>
   <sheetViews>
-    <sheetView topLeftCell="A2" workbookViewId="0">
-      <selection activeCell="C38" sqref="C37:C38"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="L10" sqref="L10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -882,9 +1018,13 @@
     <col min="1" max="1" width="13.85546875" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="15.42578125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="14.7109375" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="15.42578125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="17.28515625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="31.7109375" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="9.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -894,8 +1034,17 @@
       <c r="C1" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="G1" t="s">
+        <v>1</v>
+      </c>
+      <c r="H1" t="s">
+        <v>2</v>
+      </c>
+      <c r="J1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A2" s="1">
         <v>44562</v>
       </c>
@@ -905,8 +1054,26 @@
       <c r="C2">
         <v>0</v>
       </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="F2" t="s">
+        <v>7</v>
+      </c>
+      <c r="G2">
+        <f>(SUM(data1_simple!B2:B14,data1_simple!B18:B25)-SUM(data1_simple!B15:B17))/SUM(data1_simple!B2:B25)</f>
+        <v>0.39423076923076922</v>
+      </c>
+      <c r="H2">
+        <f>(SUM(data1_simple!C2:C14,data1_simple!C18:C25)-SUM(data1_simple!C15:C17))/SUM(data1_simple!C2:C25)</f>
+        <v>0.48247422680412372</v>
+      </c>
+      <c r="J2" t="s">
+        <v>5</v>
+      </c>
+      <c r="K2">
+        <f>G4-H4</f>
+        <v>2000</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A3" s="1">
         <v>44562.041666666664</v>
       </c>
@@ -916,8 +1083,26 @@
       <c r="C3">
         <v>0</v>
       </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="F3" t="s">
+        <v>3</v>
+      </c>
+      <c r="G3">
+        <f>AVERAGE(B2:B25)</f>
+        <v>4333.333333333333</v>
+      </c>
+      <c r="H3">
+        <f>AVERAGE(C2:C25)</f>
+        <v>4041.6666666666665</v>
+      </c>
+      <c r="J3" t="s">
+        <v>9</v>
+      </c>
+      <c r="K3" s="11">
+        <f>(G6-H6)/3</f>
+        <v>2133.3333333333335</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A4" s="1">
         <v>44562.083333333336</v>
       </c>
@@ -927,8 +1112,19 @@
       <c r="C4">
         <v>0</v>
       </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="F4" t="s">
+        <v>4</v>
+      </c>
+      <c r="G4">
+        <f>B15</f>
+        <v>10000</v>
+      </c>
+      <c r="H4">
+        <f>C15</f>
+        <v>8000</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A5" s="1">
         <v>44562.125</v>
       </c>
@@ -938,8 +1134,19 @@
       <c r="C5">
         <v>0</v>
       </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="F5" t="s">
+        <v>6</v>
+      </c>
+      <c r="G5">
+        <f>G3/G4</f>
+        <v>0.43333333333333329</v>
+      </c>
+      <c r="H5">
+        <f>H3/H4</f>
+        <v>0.50520833333333326</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A6" s="1">
         <v>44562.166666666664</v>
       </c>
@@ -949,8 +1156,19 @@
       <c r="C6">
         <v>0</v>
       </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="F6" t="s">
+        <v>10</v>
+      </c>
+      <c r="G6">
+        <f>SUM(B15:B17)</f>
+        <v>31500</v>
+      </c>
+      <c r="H6">
+        <f>SUM(C15:C17)</f>
+        <v>25100</v>
+      </c>
+    </row>
+    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A7" s="1">
         <v>44562.208333333336</v>
       </c>
@@ -961,7 +1179,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A8" s="1">
         <v>44562.25</v>
       </c>
@@ -972,7 +1190,7 @@
         <v>2400</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A9" s="1">
         <v>44562.291666666664</v>
       </c>
@@ -980,10 +1198,10 @@
         <v>3000</v>
       </c>
       <c r="C9">
-        <v>2800</v>
-      </c>
-    </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+        <v>3100</v>
+      </c>
+    </row>
+    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A10" s="1">
         <v>44562.333333333336</v>
       </c>
@@ -991,10 +1209,10 @@
         <v>3500</v>
       </c>
       <c r="C10">
-        <v>3400</v>
-      </c>
-    </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+        <v>3600</v>
+      </c>
+    </row>
+    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A11" s="1">
         <v>44562.375</v>
       </c>
@@ -1002,10 +1220,10 @@
         <v>4000</v>
       </c>
       <c r="C11">
-        <v>3800</v>
-      </c>
-    </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+        <v>3900</v>
+      </c>
+    </row>
+    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A12" s="1">
         <v>44562.416666666664</v>
       </c>
@@ -1016,7 +1234,7 @@
         <v>4400</v>
       </c>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A13" s="1">
         <v>44562.458333333336</v>
       </c>
@@ -1027,7 +1245,7 @@
         <v>4800</v>
       </c>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A14" s="1">
         <v>44562.5</v>
       </c>
@@ -1038,37 +1256,37 @@
         <v>5400</v>
       </c>
     </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A15" s="1">
+    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A15" s="4">
         <v>44562.541666666664</v>
       </c>
-      <c r="B15">
+      <c r="B15" s="5">
         <v>10000</v>
       </c>
-      <c r="C15">
-        <v>9800</v>
-      </c>
-    </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A16" s="1">
+      <c r="C15" s="6">
+        <v>8000</v>
+      </c>
+    </row>
+    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A16" s="7">
         <v>44562.583333333336</v>
       </c>
-      <c r="B16">
+      <c r="B16" s="2">
         <v>10500</v>
       </c>
-      <c r="C16">
-        <v>10400</v>
+      <c r="C16" s="8">
+        <v>8200</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A17" s="1">
+      <c r="A17" s="9">
         <v>44562.625</v>
       </c>
-      <c r="B17">
+      <c r="B17" s="3">
         <v>11000</v>
       </c>
-      <c r="C17">
-        <v>10800</v>
+      <c r="C17" s="10">
+        <v>8900</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.25">
@@ -1079,7 +1297,7 @@
         <v>9500</v>
       </c>
       <c r="C18">
-        <v>9400</v>
+        <v>9600</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.25">
@@ -1090,7 +1308,7 @@
         <v>8000</v>
       </c>
       <c r="C19">
-        <v>7800</v>
+        <v>8100</v>
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.25">
@@ -1165,38 +1383,15 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B2"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+  <dimension ref="A1"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G30" sqref="G30"/>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:B1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="15.42578125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="14.7109375" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
-        <v>1</v>
-      </c>
-      <c r="B1" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A2">
-        <f>(SUM(data1_simple!B2:B14,data1_simple!B18:B25)-SUM(data1_simple!B15:B17))/SUM(data1_simple!B2:B25)</f>
-        <v>0.39423076923076922</v>
-      </c>
-      <c r="B2">
-        <f>(SUM(data1_simple!C2:C14,data1_simple!C18:C25)-SUM(data1_simple!C15:C17))/SUM(data1_simple!C2:C25)</f>
-        <v>0.39096267190569745</v>
-      </c>
-    </row>
-  </sheetData>
+  <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>